<commit_message>
update 2020 Example Excel Book to include INFINITE upper bounds
</commit_message>
<xml_diff>
--- a/coefficients/2020/01 Example Excel Book.xlsx
+++ b/coefficients/2020/01 Example Excel Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keithrichards/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC49457E-4430-A447-AA19-58B31B8D4ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB3F39E-D706-3F40-899B-7F692CAB448A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="460" windowWidth="44080" windowHeight="23420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5140" yWindow="460" windowWidth="44080" windowHeight="23420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example Calculation" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="92">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>DASH PAIN NPRS (IROMS 20) </t>
+  </si>
+  <si>
+    <t>INFINITY</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
@@ -20319,8 +20322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20673,8 +20676,8 @@
       <c r="A9" s="1">
         <v>365.01</v>
       </c>
-      <c r="B9" s="1">
-        <v>1000000</v>
+      <c r="B9" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>80</v>

</xml_diff>